<commit_message>
Initial commit for Note 003
</commit_message>
<xml_diff>
--- a/resources/analysis/PageStatistics.xlsx
+++ b/resources/analysis/PageStatistics.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j NEW\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j NEW\resources\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC098617-C1AC-409A-BAE1-6181A01C0EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86F8F52-4D0E-4C98-96A5-12AF6620CC7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="3" r:id="rId1"/>
     <sheet name="VoynichStatsMajority" sheetId="2" r:id="rId2"/>
     <sheet name="VoynichStatsConcordance" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VoynichStatsConcordance!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VoynichStatsMajority!$A$1:$L$228</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -885,7 +889,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1736,11 +1740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,28 +1863,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -10548,34 +10552,35 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L228" xr:uid="{83B18A73-E32E-4DED-898C-F822A41E890E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -19243,6 +19248,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L1" xr:uid="{96C7D5E5-E629-4C47-9A3F-4000866015AD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed exclusion of parchment 25 from clustering
</commit_message>
<xml_diff>
--- a/resources/analysis/PageStatistics.xlsx
+++ b/resources/analysis/PageStatistics.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mzatt\Projects\Git - v4j\resources\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05977AC2-B2B6-4297-BA80-87D472A0670C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAFD43B-46BC-4FFD-AD27-BDFD2C6B9942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="807" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="3" r:id="rId1"/>
     <sheet name="VoynichStatsMajority" sheetId="2" r:id="rId2"/>
     <sheet name="VoynichStatsConcordance" sheetId="1" r:id="rId3"/>
     <sheet name="Pivot - Majority" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$B$2:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">VoynichStatsConcordance!$A$1:$L$228</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VoynichStatsMajority!$A$1:$L$228</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2945" uniqueCount="298">
   <si>
     <t>ID</t>
   </si>
@@ -889,40 +891,152 @@
     <t>Sum of ClearTokens</t>
   </si>
   <si>
-    <t>Terms</t>
-  </si>
-  <si>
-    <t>Unique "words" in page (counting those with "unreadable" characters).</t>
-  </si>
-  <si>
     <t>Total number of "word" instances in page (counting those with "unreadable" characters).</t>
   </si>
   <si>
-    <t>Unique "words" in page (counting those with NO "unreadable" characters).</t>
-  </si>
-  <si>
     <t>Total number of "word" instances in page (counting those with NO "unreadable" characters).</t>
   </si>
   <si>
     <t>(also see https://mzattera.github.io/v4j/)</t>
   </si>
   <si>
-    <t>ClearTerms</t>
-  </si>
-  <si>
     <t>v4j cluster (see https://mzattera.github.io/v4j/003/).</t>
   </si>
   <si>
-    <t>ClearTems</t>
-  </si>
-  <si>
-    <t>Sum of Terms</t>
-  </si>
-  <si>
-    <t>Sum of ClearTems</t>
-  </si>
-  <si>
     <t>Count of ID</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Unique word types in page (counting those with "unreadable" characters).</t>
+  </si>
+  <si>
+    <t>Unique word types in page (counting those with NO "unreadable" characters).</t>
+  </si>
+  <si>
+    <t>ClearTypes</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Biological)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Herbal A)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Herbal B)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Pharmaceutical)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Stars)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pages</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,8 +1377,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1379,6 +1505,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1424,7 +1661,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1435,6 +1672,38 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1480,42 +1749,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1565,7 +1799,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Massimiliano Zattera" refreshedDate="44745.369474884261" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="227" xr:uid="{AA1FB498-4F86-4D3F-9E3C-B3368C6A2667}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Massimiliano Zattera" refreshedDate="44834.394108680557" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="227" xr:uid="{AA1FB498-4F86-4D3F-9E3C-B3368C6A2667}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:L228" sheet="VoynichStatsMajority"/>
   </cacheSource>
@@ -1606,13 +1840,13 @@
     <cacheField name="Tokens" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="606"/>
     </cacheField>
-    <cacheField name="Terms" numFmtId="0">
+    <cacheField name="Types" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="364"/>
     </cacheField>
     <cacheField name="ClearTokens" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="595"/>
     </cacheField>
-    <cacheField name="ClearTems" numFmtId="0">
+    <cacheField name="ClearTypes" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="355"/>
     </cacheField>
   </cacheFields>
@@ -2946,7 +3180,7 @@
     <s v="f49r"/>
     <s v="H"/>
     <s v="A"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <s v="G"/>
     <s v="A"/>
@@ -2960,7 +3194,7 @@
     <s v="f49v"/>
     <s v="H"/>
     <s v="A"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <s v="G"/>
     <s v="B"/>
@@ -3142,7 +3376,7 @@
     <s v="f56r"/>
     <s v="H"/>
     <s v="A"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <s v="G"/>
     <s v="O"/>
@@ -3156,7 +3390,7 @@
     <s v="f56v"/>
     <s v="H"/>
     <s v="A"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="1"/>
     <s v="G"/>
     <s v="P"/>
@@ -4808,8 +5042,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD0DA326-6ECD-41DF-8367-E78B15CBFE45}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD0DA326-6ECD-41DF-8367-E78B15CBFE45}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -4831,9 +5065,9 @@
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="3"/>
@@ -4864,7 +5098,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="5">
+  <colItems count="3">
     <i>
       <x/>
     </i>
@@ -4874,34 +5108,26 @@
     <i i="2">
       <x v="2"/>
     </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
   </colItems>
-  <dataFields count="5">
+  <dataFields count="3">
     <dataField name="Sum of Tokens" fld="8" baseField="0" baseItem="0"/>
     <dataField name="Sum of ClearTokens" fld="10" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Terms" fld="9" baseField="0" baseItem="0"/>
-    <dataField name="Sum of ClearTems" fld="11" baseField="0" baseItem="0"/>
     <dataField name="Count of ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="9">
+    <format dxfId="4">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="AA1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="3">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="AC1" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="2">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="AD1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="1">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="AL1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="0">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="AB1" fieldPosition="0"/>
     </format>
   </formats>
@@ -5220,7 +5446,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5266,7 +5492,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5303,10 +5529,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5314,15 +5540,15 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B12" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5330,12 +5556,12 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -5348,8 +5574,8 @@
   <dimension ref="A1:L228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,7 +5623,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
@@ -8989,7 +9215,7 @@
         <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -9027,7 +9253,7 @@
         <v>12</v>
       </c>
       <c r="D97" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -9521,7 +9747,7 @@
         <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -9559,7 +9785,7 @@
         <v>12</v>
       </c>
       <c r="D111" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -14033,7 +14259,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L228" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -14044,8 +14269,8 @@
   <dimension ref="A1:L228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14093,7 +14318,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>9</v>
@@ -17685,7 +17910,7 @@
         <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -17723,7 +17948,7 @@
         <v>12</v>
       </c>
       <c r="D97" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -18217,7 +18442,7 @@
         <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -18255,7 +18480,7 @@
         <v>12</v>
       </c>
       <c r="D111" t="s">
-        <v>139</v>
+        <v>276</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -22741,8 +22966,8 @@
   </sheetPr>
   <dimension ref="A3:AO43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22750,7 +22975,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
@@ -22799,13 +23024,7 @@
         <v>281</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E3" t="s">
-        <v>292</v>
-      </c>
-      <c r="F3" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -22818,19 +23037,13 @@
         <v>139</v>
       </c>
       <c r="B4" s="7">
-        <v>7639</v>
+        <v>7172</v>
       </c>
       <c r="C4" s="7">
-        <v>6678</v>
+        <v>6225</v>
       </c>
       <c r="D4" s="7">
-        <v>5847</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4943</v>
-      </c>
-      <c r="F4" s="7">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AD4"/>
       <c r="AE4"/>
@@ -22849,12 +23062,6 @@
         <v>6804</v>
       </c>
       <c r="D5" s="7">
-        <v>3771</v>
-      </c>
-      <c r="E5" s="7">
-        <v>3597</v>
-      </c>
-      <c r="F5" s="7">
         <v>20</v>
       </c>
       <c r="AD5"/>
@@ -22868,19 +23075,13 @@
         <v>276</v>
       </c>
       <c r="B6" s="7">
-        <v>7315</v>
+        <v>7782</v>
       </c>
       <c r="C6" s="7">
-        <v>7156</v>
+        <v>7609</v>
       </c>
       <c r="D6" s="7">
-        <v>5919</v>
-      </c>
-      <c r="E6" s="7">
-        <v>5760</v>
-      </c>
-      <c r="F6" s="7">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AD6"/>
       <c r="AE6"/>
@@ -22899,12 +23100,6 @@
         <v>3159</v>
       </c>
       <c r="D7" s="7">
-        <v>2605</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2533</v>
-      </c>
-      <c r="F7" s="7">
         <v>30</v>
       </c>
       <c r="AD7"/>
@@ -22924,12 +23119,6 @@
         <v>2390</v>
       </c>
       <c r="D8" s="7">
-        <v>1991</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1818</v>
-      </c>
-      <c r="F8" s="7">
         <v>16</v>
       </c>
       <c r="AD8"/>
@@ -22949,12 +23138,6 @@
         <v>10399</v>
       </c>
       <c r="D9" s="7">
-        <v>6808</v>
-      </c>
-      <c r="E9" s="7">
-        <v>6486</v>
-      </c>
-      <c r="F9" s="7">
         <v>23</v>
       </c>
       <c r="AD9"/>
@@ -22974,12 +23157,6 @@
         <v>36586</v>
       </c>
       <c r="D10" s="7">
-        <v>26941</v>
-      </c>
-      <c r="E10" s="7">
-        <v>25137</v>
-      </c>
-      <c r="F10" s="7">
         <v>227</v>
       </c>
       <c r="AD10"/>
@@ -23060,4 +23237,142 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD47481-B07D-4AAE-A234-6E06E725CA9C}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="11.42578125" style="8" customWidth="1"/>
+    <col min="5" max="6" width="20.85546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10726</v>
+      </c>
+      <c r="D3" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="15">
+        <v>7782</v>
+      </c>
+      <c r="D4" s="16">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="15">
+        <v>6981</v>
+      </c>
+      <c r="D5" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="15">
+        <v>3231</v>
+      </c>
+      <c r="D6" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2577</v>
+      </c>
+      <c r="D7" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="15">
+        <v>7172</v>
+      </c>
+      <c r="D8" s="16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18">
+        <v>38469</v>
+      </c>
+      <c r="D9" s="19">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="9" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>